<commit_message>
msi and portable exe created
</commit_message>
<xml_diff>
--- a/Database/Book2.xlsx
+++ b/Database/Book2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>Name</t>
   </si>
@@ -295,9 +295,6 @@
     <t>اسكينول منظف وجة 225 مل</t>
   </si>
   <si>
-    <t>اسمارت بيبى حلمة 36 ق</t>
-  </si>
-  <si>
     <t>اسيتون 250 مل Byphasse</t>
   </si>
   <si>
@@ -317,6 +314,12 @@
   </si>
   <si>
     <t>اصالة حنة اكسترا الوان</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>aa</t>
   </si>
 </sst>
 </file>
@@ -674,7 +677,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1959,10 +1962,10 @@
         <v>93</v>
       </c>
       <c r="C92">
-        <v>2.5</v>
+        <v>49.9</v>
       </c>
       <c r="D92">
-        <v>55</v>
+        <v>35.99</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1973,10 +1976,10 @@
         <v>94</v>
       </c>
       <c r="C93">
-        <v>49.9</v>
+        <v>16</v>
       </c>
       <c r="D93">
-        <v>35.99</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1987,10 +1990,10 @@
         <v>95</v>
       </c>
       <c r="C94">
-        <v>16</v>
+        <v>2.5</v>
       </c>
       <c r="D94">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2001,10 +2004,10 @@
         <v>96</v>
       </c>
       <c r="C95">
-        <v>2.5</v>
+        <v>36</v>
       </c>
       <c r="D95">
-        <v>35</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2015,10 +2018,10 @@
         <v>97</v>
       </c>
       <c r="C96">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D96">
-        <v>25.2</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2029,10 +2032,10 @@
         <v>98</v>
       </c>
       <c r="C97">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="D97">
-        <v>15.5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2043,10 +2046,10 @@
         <v>99</v>
       </c>
       <c r="C98">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="D98">
-        <v>45</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2057,10 +2060,24 @@
         <v>100</v>
       </c>
       <c r="C99">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D99">
-        <v>9.5</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>101</v>
+      </c>
+      <c r="C100">
+        <v>3</v>
+      </c>
+      <c r="D100">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>